<commit_message>
bugfix: Fix renaming portfolio na account and change logic to str
</commit_message>
<xml_diff>
--- a/data/phemex_futures_trades.xlsx
+++ b/data/phemex_futures_trades.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TradesLong" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t xml:space="preserve">Asset</t>
   </si>
@@ -53,9 +53,6 @@
     <t xml:space="preserve">Tier 3</t>
   </si>
   <si>
-    <t xml:space="preserve">PT 70%</t>
-  </si>
-  <si>
     <t xml:space="preserve">SL 80%</t>
   </si>
   <si>
@@ -71,7 +68,7 @@
     <t xml:space="preserve">BTCUSDT</t>
   </si>
   <si>
-    <t xml:space="preserve">P1</t>
+    <t xml:space="preserve">A1</t>
   </si>
 </sst>
 </file>
@@ -250,17 +247,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -306,13 +304,10 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>18000</v>
@@ -346,13 +341,10 @@
         <v>0</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>20140</v>
-      </c>
-      <c r="L2" s="0" t="n">
         <v>19840</v>
       </c>
-      <c r="N2" s="0" t="s">
-        <v>16</v>
+      <c r="M2" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -371,13 +363,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -422,13 +414,10 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>70000</v>
@@ -462,13 +451,10 @@
         <v>0</v>
       </c>
       <c r="K2" s="0" t="n">
-        <v>20140</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <v>19840</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>16</v>
+        <v>70060</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: renaming and fixing phemex tickers and corecting placing trades with prefix 10, 100, 1000, 10000, 100000, 1000000, ....
</commit_message>
<xml_diff>
--- a/data/phemex_futures_trades.xlsx
+++ b/data/phemex_futures_trades.xlsx
@@ -21,11 +21,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
   <si>
     <t xml:space="preserve">Asset</t>
   </si>
   <si>
+    <t xml:space="preserve">Last Price</t>
+  </si>
+  <si>
     <t xml:space="preserve">Entry price</t>
   </si>
   <si>
@@ -41,22 +44,13 @@
     <t xml:space="preserve">Leverage</t>
   </si>
   <si>
-    <t xml:space="preserve">PossibleTrade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tier 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tier 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tier 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SL 80%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CreateDate</t>
+    <t xml:space="preserve">Move</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tier</t>
   </si>
   <si>
     <t xml:space="preserve">On exchange</t>
@@ -65,7 +59,7 @@
     <t xml:space="preserve">Note</t>
   </si>
   <si>
-    <t xml:space="preserve">BTCUSDPERP</t>
+    <t xml:space="preserve">uBTCUSD</t>
   </si>
   <si>
     <t xml:space="preserve">A1</t>
@@ -247,18 +241,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -298,59 +293,37 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>18000</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>17900</v>
+        <v>15000</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>20200</v>
+        <v>14900</v>
       </c>
       <c r="E2" s="0" t="n">
+        <v>17200</v>
+      </c>
+      <c r="F2" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="G2" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="G2" s="2" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H2" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>19840</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>15</v>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -366,10 +339,16 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="O4" activeCellId="0" sqref="O4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.17"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -408,59 +387,39 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C2" s="0" t="n">
         <v>70000</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="D2" s="0" t="n">
         <v>70100</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="E2" s="0" t="n">
         <v>68000</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="F2" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="G2" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="G2" s="2" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="H2" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>70060</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>15</v>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>